<commit_message>
Test finished and last bug fixed on the method turnFaceRight
</commit_message>
<xml_diff>
--- a/src/com/martdel/rubik/schema.xlsx
+++ b/src/com/martdel/rubik/schema.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MartDel\Desktop\programmation\Java\rubik\src\com\martdel\rubik\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8851475A-113F-4593-8170-3754DA1B0470}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B72480C6-230C-4784-B9A7-1354F8905749}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="480" windowWidth="24240" windowHeight="13140" xr2:uid="{B117DAF9-EA99-4BEA-8465-1CDD5ECE0916}"/>
   </bookViews>
@@ -937,7 +937,7 @@
   <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1118,13 +1118,13 @@
       <c r="A8" s="1"/>
       <c r="B8" s="2"/>
       <c r="C8" s="7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D8" s="7">
         <v>2</v>
       </c>
       <c r="E8" s="7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F8" s="5"/>
       <c r="G8" s="6"/>
@@ -1282,25 +1282,25 @@
       <c r="A14" s="1"/>
       <c r="B14" s="2"/>
       <c r="C14" s="7">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D14" s="7">
         <v>5</v>
       </c>
       <c r="E14" s="7">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="F14" s="5"/>
       <c r="G14" s="6"/>
       <c r="H14" s="2"/>
       <c r="I14" s="3">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="J14" s="4">
         <v>7</v>
       </c>
       <c r="K14" s="4">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="L14" s="5"/>
     </row>

</xml_diff>